<commit_message>
Updated BOM and added more 3D models
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="81">
   <si>
     <t>GBP to USD</t>
   </si>
@@ -71,7 +71,7 @@
     <t>reprapworld.com</t>
   </si>
   <si>
-    <t>One rod will be cut in half</t>
+    <t>Two will be cut in half</t>
   </si>
   <si>
     <t>LM10UU</t>
@@ -83,18 +83,6 @@
     <t>robotdigg.com</t>
   </si>
   <si>
-    <t>Slider rail 16mm - 40cm</t>
-  </si>
-  <si>
-    <t>Guide rail for gantry Y-Axis</t>
-  </si>
-  <si>
-    <t>Slider - 16mm</t>
-  </si>
-  <si>
-    <t>Linear bearings for 16 mm slider rails;</t>
-  </si>
-  <si>
     <t>M10 Threaded rod - 100cm</t>
   </si>
   <si>
@@ -125,7 +113,22 @@
     <t>Rostock 16 Teeth 5mm Bore GT2 Pulley</t>
   </si>
   <si>
-    <t>GT2 pulley for X-Y motion</t>
+    <t>GT2 pulley for X-Y motion steppers</t>
+  </si>
+  <si>
+    <t>2GT 20 Tooth 6.35mm Bore Pulley</t>
+  </si>
+  <si>
+    <t>GT2 pulley for gantry idlers</t>
+  </si>
+  <si>
+    <t>#10-24 binding post barrel</t>
+  </si>
+  <si>
+    <t>fastenal.com</t>
+  </si>
+  <si>
+    <t>#10-24 binding post male shoulder screw</t>
   </si>
   <si>
     <t>GT2-B6</t>
@@ -179,16 +182,10 @@
     <t>M6-1.0 x 16 mm machine screws; for frame assembly</t>
   </si>
   <si>
-    <t>fastenal.com</t>
-  </si>
-  <si>
-    <t>QM2530016A20000 </t>
-  </si>
-  <si>
-    <t>M4-0.7 x 16 mm machine screws; for stepper motors</t>
-  </si>
-  <si>
-    <t>M4 fender washers</t>
+    <t>M3-0.5 x 16 mm machine screws; for stepper motors</t>
+  </si>
+  <si>
+    <t>M3 fender washers</t>
   </si>
   <si>
     <t>WC6360000A20000 </t>
@@ -358,7 +355,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -428,11 +425,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -468,10 +473,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -606,11 +611,11 @@
         <v>5.4264</v>
       </c>
       <c r="F7" s="11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" s="14" t="n">
         <f aca="false">F7*E7</f>
-        <v>16.2792</v>
+        <v>21.7056</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>17</v>
@@ -632,11 +637,11 @@
         <v>8</v>
       </c>
       <c r="F8" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="14" t="n">
         <f aca="false">F8*E8</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>21</v>
@@ -652,18 +657,18 @@
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="12" t="n">
-        <v>12.99</v>
+        <v>2.99</v>
       </c>
       <c r="E9" s="14" t="n">
         <f aca="false">D9*D2</f>
-        <v>17.6664</v>
+        <v>4.0664</v>
       </c>
       <c r="F9" s="11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="14" t="n">
         <f aca="false">F9*E9</f>
-        <v>35.3328</v>
+        <v>4.0664</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>17</v>
@@ -679,18 +684,18 @@
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="12" t="n">
-        <v>3.99</v>
+        <v>14.99</v>
       </c>
       <c r="E10" s="14" t="n">
         <f aca="false">D10*D2</f>
-        <v>5.4264</v>
+        <v>20.3864</v>
       </c>
       <c r="F10" s="11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G10" s="14" t="n">
         <f aca="false">F10*E10</f>
-        <v>21.7056</v>
+        <v>20.3864</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>17</v>
@@ -706,18 +711,18 @@
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="12" t="n">
-        <v>2.99</v>
+        <v>4.49</v>
       </c>
       <c r="E11" s="14" t="n">
         <f aca="false">D11*D2</f>
-        <v>4.0664</v>
+        <v>6.1064</v>
       </c>
       <c r="F11" s="11" t="n">
         <v>1</v>
       </c>
       <c r="G11" s="14" t="n">
         <f aca="false">F11*E11</f>
-        <v>4.0664</v>
+        <v>6.1064</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>17</v>
@@ -725,62 +730,56 @@
       <c r="I11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="10" t="n">
+        <v>70780</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="C12" s="13"/>
-      <c r="D12" s="12" t="n">
-        <v>14.99</v>
-      </c>
-      <c r="E12" s="14" t="n">
-        <f aca="false">D12*D2</f>
-        <v>20.3864</v>
+      <c r="D12" s="13"/>
+      <c r="E12" s="16" t="n">
+        <v>35</v>
       </c>
       <c r="F12" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="14" t="n">
         <f aca="false">F12*E12</f>
-        <v>20.3864</v>
+        <v>70</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="10" t="n">
+        <v>38832</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="C13" s="13"/>
-      <c r="D13" s="12" t="n">
-        <v>4.49</v>
-      </c>
-      <c r="E13" s="14" t="n">
-        <f aca="false">D13*D2</f>
-        <v>6.1064</v>
+      <c r="D13" s="13"/>
+      <c r="E13" s="16" t="n">
+        <v>3.8</v>
       </c>
       <c r="F13" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="14" t="n">
         <f aca="false">F13*E13</f>
-        <v>6.1064</v>
+        <v>7.6</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
-        <v>70780</v>
+      <c r="A14" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>32</v>
@@ -788,241 +787,241 @@
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="16" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="F14" s="11" t="n">
         <v>2</v>
       </c>
       <c r="G14" s="14" t="n">
         <f aca="false">F14*E14</f>
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="15"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="n">
-        <v>38832</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="16" t="n">
-        <v>3.8</v>
+        <v>2</v>
       </c>
       <c r="F15" s="11" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G15" s="14" t="n">
         <f aca="false">F15*E15</f>
-        <v>7.6</v>
+        <v>16</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I15" s="15"/>
     </row>
-    <row r="16" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18" t="n">
+        <v>123383</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="16" t="n">
-        <v>2</v>
+        <v>1.18</v>
       </c>
       <c r="F16" s="11" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G16" s="14" t="n">
         <f aca="false">F16*E16</f>
-        <v>20</v>
+        <v>9.44</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="19" t="n">
+        <v>11129031</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="16" t="n">
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="F17" s="11" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G17" s="14" t="n">
         <f aca="false">F17*E17</f>
         <v>10</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>39</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="16" t="n">
-        <v>0.35</v>
+        <v>2</v>
       </c>
       <c r="F18" s="11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G18" s="14" t="n">
         <f aca="false">F18*E18</f>
-        <v>0.35</v>
+        <v>10</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="15"/>
+      <c r="I18" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="16" t="n">
-        <v>13.6</v>
+        <v>0.35</v>
       </c>
       <c r="F19" s="11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G19" s="14" t="n">
         <f aca="false">F19*E19</f>
-        <v>54.4</v>
+        <v>0.35</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="I19" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="16" t="n">
-        <v>6.8</v>
+        <v>13.6</v>
       </c>
       <c r="F20" s="11" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G20" s="14" t="n">
         <f aca="false">F20*E20</f>
         <v>54.4</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="16" t="n">
-        <v>5.44</v>
+        <v>6.8</v>
       </c>
       <c r="F21" s="11" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G21" s="14" t="n">
         <f aca="false">F21*E21</f>
-        <v>10.88</v>
+        <v>54.4</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I21" s="15"/>
     </row>
     <row r="22" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="16" t="n">
-        <v>4.08</v>
+        <v>5.44</v>
       </c>
       <c r="F22" s="11" t="n">
         <v>2</v>
       </c>
       <c r="G22" s="14" t="n">
         <f aca="false">F22*E22</f>
-        <v>8.16</v>
+        <v>10.88</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I22" s="15"/>
     </row>
     <row r="23" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="16" t="n">
-        <v>33.24</v>
+        <v>4.08</v>
       </c>
       <c r="F23" s="11" t="n">
         <v>2</v>
       </c>
       <c r="G23" s="14" t="n">
         <f aca="false">F23*E23</f>
-        <v>66.48</v>
+        <v>8.16</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I23" s="15"/>
     </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="n">
-        <v>91234</v>
+    <row r="24" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>53</v>
@@ -1030,109 +1029,119 @@
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="16" t="n">
-        <v>0.1368</v>
+        <v>33.24</v>
       </c>
       <c r="F24" s="11" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G24" s="14" t="n">
         <f aca="false">F24*E24</f>
-        <v>16.416</v>
+        <v>66.48</v>
       </c>
       <c r="H24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="18" t="n">
+        <v>91234</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="I24" s="15"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>56</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="14" t="n">
-        <v>0.0848</v>
-      </c>
-      <c r="F25" s="15" t="n">
-        <v>20</v>
+      <c r="E25" s="16" t="n">
+        <v>0.1368</v>
+      </c>
+      <c r="F25" s="11" t="n">
+        <v>120</v>
       </c>
       <c r="G25" s="14" t="n">
         <f aca="false">F25*E25</f>
-        <v>1.696</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>54</v>
+        <v>16.416</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="I25" s="15"/>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="n">
-        <v>11511782</v>
+    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="20" t="n">
+        <v>91191</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="14" t="n">
-        <v>0.054</v>
+        <v>0.0436</v>
       </c>
       <c r="F26" s="15" t="n">
-        <f aca="false">F25</f>
         <v>20</v>
       </c>
       <c r="G26" s="14" t="n">
         <f aca="false">F26*E26</f>
-        <v>1.08</v>
+        <v>0.872</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="I26" s="15"/>
     </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>58</v>
+    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="20" t="n">
+        <v>110751</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="14" t="n">
-        <v>0.0888</v>
+        <v>0.054</v>
       </c>
       <c r="F27" s="15" t="n">
-        <v>120</v>
+        <f aca="false">F26</f>
+        <v>20</v>
       </c>
       <c r="G27" s="14" t="n">
         <f aca="false">F27*E27</f>
-        <v>10.656</v>
+        <v>1.08</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="I27" s="15"/>
     </row>
-    <row r="28" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="19"/>
-      <c r="B28" s="15"/>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
+      <c r="E28" s="14" t="n">
+        <v>0.0888</v>
+      </c>
+      <c r="F28" s="15" t="n">
+        <v>120</v>
+      </c>
       <c r="G28" s="14" t="n">
         <f aca="false">F28*E28</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="15"/>
+        <v>10.656</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>36</v>
+      </c>
       <c r="I28" s="15"/>
     </row>
     <row r="29" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="15"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -1146,7 +1155,7 @@
       <c r="I29" s="15"/>
     </row>
     <row r="30" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="15"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
@@ -1174,151 +1183,141 @@
       <c r="I31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="14" t="n">
+        <f aca="false">F32*E32</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6"/>
-      <c r="F33" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="G33" s="21" t="n">
-        <f aca="false">SUM(G6:G31)</f>
-        <v>603.7948</v>
-      </c>
     </row>
     <row r="34" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6"/>
+      <c r="F34" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34" s="23" t="n">
+        <f aca="false">SUM(G6:G32)</f>
+        <v>578.7988</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
+      <c r="B39" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="C39" s="13"/>
+      <c r="D39" s="12" t="n">
+        <v>79.99</v>
+      </c>
+      <c r="E39" s="14" t="n">
+        <f aca="false">D39*D2</f>
+        <v>108.7864</v>
+      </c>
+      <c r="F39" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" s="24" t="n">
+        <f aca="false">F39*E39</f>
+        <v>108.7864</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="15"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="n">
+        <v>2133</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="12" t="n">
-        <v>79.99</v>
-      </c>
-      <c r="E38" s="14" t="n">
-        <f aca="false">D38*D2</f>
-        <v>108.7864</v>
-      </c>
-      <c r="F38" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G38" s="22" t="n">
-        <f aca="false">F38*E38</f>
-        <v>108.7864</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I38" s="15"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="n">
-        <v>2133</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="16" t="n">
-        <v>13.95</v>
-      </c>
-      <c r="F39" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G39" s="22" t="n">
-        <f aca="false">F39*E39</f>
-        <v>69.75</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I39" s="15"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
       <c r="E40" s="16" t="n">
-        <v>11.8</v>
+        <v>13.95</v>
       </c>
       <c r="F40" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="G40" s="22" t="n">
+      <c r="G40" s="24" t="n">
         <f aca="false">F40*E40</f>
+        <v>69.75</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I40" s="15"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="16" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="F41" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G41" s="24" t="n">
+        <f aca="false">F41*E41</f>
         <v>59</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I40" s="15"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="16" t="n">
-        <v>20</v>
-      </c>
-      <c r="F41" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G41" s="22" t="n">
-        <f aca="false">F41*E41</f>
-        <v>20</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>21</v>
@@ -1326,212 +1325,222 @@
       <c r="I41" s="15"/>
     </row>
     <row r="42" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="n">
+      <c r="A42" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="F42" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="24" t="n">
+        <f aca="false">F42*E42</f>
+        <v>20</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="15"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="10" t="n">
         <v>1405</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="16" t="n">
+      <c r="B43" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="16" t="n">
         <v>0.75</v>
-      </c>
-      <c r="F42" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G42" s="22" t="n">
-        <f aca="false">F42*E42</f>
-        <v>3.75</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I42" s="15"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="12" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="E43" s="14" t="n">
-        <f aca="false">D43*D2</f>
-        <v>1.7</v>
       </c>
       <c r="F43" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="G43" s="22" t="n">
+      <c r="G43" s="24" t="n">
         <f aca="false">F43*E43</f>
+        <v>3.75</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I43" s="15"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="12" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E44" s="14" t="n">
+        <f aca="false">D44*D2</f>
+        <v>1.7</v>
+      </c>
+      <c r="F44" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G44" s="24" t="n">
+        <f aca="false">F44*E44</f>
         <v>8.5</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I43" s="15"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="n">
+      <c r="I44" s="15"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="n">
         <v>26171</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="16" t="n">
-        <v>12</v>
-      </c>
-      <c r="F44" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="G44" s="22" t="n">
-        <f aca="false">F44*E44</f>
-        <v>24</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I44" s="15"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="B45" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
       <c r="E45" s="16" t="n">
-        <v>64.99</v>
+        <v>12</v>
       </c>
       <c r="F45" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G45" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="G45" s="24" t="n">
         <f aca="false">F45*E45</f>
-        <v>64.99</v>
+        <v>24</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="I45" s="15"/>
     </row>
     <row r="46" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10" t="n">
-        <v>1902</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>77</v>
+      <c r="A46" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="14" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="F46" s="15" t="n">
+      <c r="E46" s="16" t="n">
+        <v>64.99</v>
+      </c>
+      <c r="F46" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="G46" s="22" t="n">
+      <c r="G46" s="24" t="n">
         <f aca="false">F46*E46</f>
-        <v>0.79</v>
+        <v>64.99</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="I46" s="15"/>
     </row>
     <row r="47" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="n">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
       <c r="E47" s="14" t="n">
-        <v>0.59</v>
+        <v>0.79</v>
       </c>
       <c r="F47" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G47" s="22" t="n">
+      <c r="G47" s="24" t="n">
         <f aca="false">F47*E47</f>
-        <v>0.59</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>65</v>
+        <v>0.79</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="I47" s="15"/>
     </row>
     <row r="48" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="n">
-        <v>1901</v>
+        <v>1903</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
       <c r="E48" s="14" t="n">
-        <v>0.69</v>
+        <v>0.59</v>
       </c>
       <c r="F48" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G48" s="22" t="n">
+      <c r="G48" s="24" t="n">
         <f aca="false">F48*E48</f>
-        <v>0.69</v>
+        <v>0.59</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I48" s="15"/>
     </row>
     <row r="49" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="n">
-        <v>1930</v>
+        <v>1901</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
       <c r="E49" s="14" t="n">
-        <v>5.95</v>
+        <v>0.69</v>
       </c>
       <c r="F49" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G49" s="22" t="n">
+      <c r="G49" s="24" t="n">
         <f aca="false">F49*E49</f>
-        <v>5.95</v>
+        <v>0.69</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I49" s="15"/>
     </row>
     <row r="50" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="10"/>
-      <c r="B50" s="15"/>
+      <c r="A50" s="10" t="n">
+        <v>1930</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="22" t="n">
+      <c r="E50" s="14" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="F50" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" s="24" t="n">
         <f aca="false">F50*E50</f>
-        <v>0</v>
-      </c>
-      <c r="H50" s="15"/>
+        <v>5.95</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="I50" s="15"/>
     </row>
     <row r="51" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1541,7 +1550,7 @@
       <c r="D51" s="13"/>
       <c r="E51" s="14"/>
       <c r="F51" s="15"/>
-      <c r="G51" s="22" t="n">
+      <c r="G51" s="24" t="n">
         <f aca="false">F51*E51</f>
         <v>0</v>
       </c>
@@ -1555,7 +1564,7 @@
       <c r="D52" s="13"/>
       <c r="E52" s="14"/>
       <c r="F52" s="15"/>
-      <c r="G52" s="22" t="n">
+      <c r="G52" s="24" t="n">
         <f aca="false">F52*E52</f>
         <v>0</v>
       </c>
@@ -1569,7 +1578,7 @@
       <c r="D53" s="13"/>
       <c r="E53" s="14"/>
       <c r="F53" s="15"/>
-      <c r="G53" s="22" t="n">
+      <c r="G53" s="24" t="n">
         <f aca="false">F53*E53</f>
         <v>0</v>
       </c>
@@ -1583,7 +1592,7 @@
       <c r="D54" s="13"/>
       <c r="E54" s="14"/>
       <c r="F54" s="15"/>
-      <c r="G54" s="22" t="n">
+      <c r="G54" s="24" t="n">
         <f aca="false">F54*E54</f>
         <v>0</v>
       </c>
@@ -1597,7 +1606,7 @@
       <c r="D55" s="13"/>
       <c r="E55" s="14"/>
       <c r="F55" s="15"/>
-      <c r="G55" s="22" t="n">
+      <c r="G55" s="24" t="n">
         <f aca="false">F55*E55</f>
         <v>0</v>
       </c>
@@ -1605,29 +1614,43 @@
       <c r="I55" s="15"/>
     </row>
     <row r="56" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="24" t="n">
+        <f aca="false">F56*E56</f>
+        <v>0</v>
+      </c>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
     </row>
     <row r="57" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6"/>
-      <c r="F57" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="G57" s="21" t="n">
-        <f aca="false">SUM(G38:G55)</f>
-        <v>366.7964</v>
-      </c>
     </row>
     <row r="58" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6"/>
+      <c r="F58" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G58" s="23" t="n">
+        <f aca="false">SUM(G39:G56)</f>
+        <v>366.7964</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6"/>
-      <c r="F59" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="G59" s="21" t="n">
-        <f aca="false">G57+G33</f>
-        <v>970.5912</v>
+    </row>
+    <row r="60" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="6"/>
+      <c r="F60" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G60" s="23" t="n">
+        <f aca="false">G58+G34</f>
+        <v>945.5952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed folder structure and updated parts list
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>GBP to USD</t>
   </si>
@@ -71,7 +71,7 @@
     <t>reprapworld.com</t>
   </si>
   <si>
-    <t>Two will be cut in half</t>
+    <t>Will be cut to length</t>
   </si>
   <si>
     <t>LM10UU</t>
@@ -149,16 +149,22 @@
     <t>GFS6-3030-1000</t>
   </si>
   <si>
-    <t>T-slotted aluminum extrusions for Z-Axis</t>
+    <t>T-slotted aluminum extrusions for Z-Axis of frame</t>
   </si>
   <si>
     <t>us.misumi-ec.com</t>
   </si>
   <si>
+    <t>GFS6-3030-600</t>
+  </si>
+  <si>
+    <t>T-slotted aluminum extrusions for X-Axis of frame</t>
+  </si>
+  <si>
     <t>GFS6-3030-500</t>
   </si>
   <si>
-    <t>T-slotted aluminum extrusions for X and Y-Axis frame and X-Axis of bed frame</t>
+    <t>T-slotted aluminum extrusions for Y-Axis of frame</t>
   </si>
   <si>
     <t>GFS6-3030-400</t>
@@ -473,10 +479,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -957,14 +963,14 @@
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="16" t="n">
-        <v>6.8</v>
+        <v>8.16</v>
       </c>
       <c r="F21" s="11" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G21" s="14" t="n">
         <f aca="false">F21*E21</f>
-        <v>54.4</v>
+        <v>32.64</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>45</v>
@@ -981,14 +987,14 @@
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="16" t="n">
-        <v>5.44</v>
+        <v>6.8</v>
       </c>
       <c r="F22" s="11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G22" s="14" t="n">
         <f aca="false">F22*E22</f>
-        <v>10.88</v>
+        <v>27.2</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>45</v>
@@ -1005,14 +1011,14 @@
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="16" t="n">
-        <v>4.08</v>
+        <v>5.44</v>
       </c>
       <c r="F23" s="11" t="n">
         <v>2</v>
       </c>
       <c r="G23" s="14" t="n">
         <f aca="false">F23*E23</f>
-        <v>8.16</v>
+        <v>10.88</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>45</v>
@@ -1029,96 +1035,95 @@
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="16" t="n">
-        <v>33.24</v>
+        <v>4.08</v>
       </c>
       <c r="F24" s="11" t="n">
         <v>2</v>
       </c>
       <c r="G24" s="14" t="n">
         <f aca="false">F24*E24</f>
-        <v>66.48</v>
+        <v>8.16</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>45</v>
       </c>
       <c r="I24" s="15"/>
     </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18" t="n">
-        <v>91234</v>
+    <row r="25" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
       <c r="E25" s="16" t="n">
-        <v>0.1368</v>
+        <v>33.24</v>
       </c>
       <c r="F25" s="11" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="G25" s="14" t="n">
         <f aca="false">F25*E25</f>
-        <v>16.416</v>
+        <v>66.48</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="I25" s="15"/>
     </row>
-    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="n">
-        <v>91191</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>55</v>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="18" t="n">
+        <v>91234</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="14" t="n">
-        <v>0.0436</v>
-      </c>
-      <c r="F26" s="15" t="n">
-        <v>20</v>
+      <c r="E26" s="16" t="n">
+        <v>0.1368</v>
+      </c>
+      <c r="F26" s="11" t="n">
+        <v>120</v>
       </c>
       <c r="G26" s="14" t="n">
         <f aca="false">F26*E26</f>
-        <v>0.872</v>
-      </c>
-      <c r="H26" s="15" t="s">
+        <v>16.416</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I26" s="15"/>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="20" t="n">
-        <v>110751</v>
+        <v>91191</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="14" t="n">
-        <v>0.054</v>
+        <v>0.0436</v>
       </c>
       <c r="F27" s="15" t="n">
-        <f aca="false">F26</f>
         <v>20</v>
       </c>
       <c r="G27" s="14" t="n">
         <f aca="false">F27*E27</f>
-        <v>1.08</v>
+        <v>0.872</v>
       </c>
       <c r="H27" s="15" t="s">
         <v>36</v>
       </c>
       <c r="I27" s="15"/>
     </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="21" t="s">
-        <v>57</v>
+    <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="20" t="n">
+        <v>110751</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>58</v>
@@ -1126,32 +1131,43 @@
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="14" t="n">
-        <v>0.0888</v>
+        <v>0.054</v>
       </c>
       <c r="F28" s="15" t="n">
-        <v>120</v>
+        <f aca="false">F27</f>
+        <v>20</v>
       </c>
       <c r="G28" s="14" t="n">
         <f aca="false">F28*E28</f>
-        <v>10.656</v>
+        <v>1.08</v>
       </c>
       <c r="H28" s="15" t="s">
         <v>36</v>
       </c>
       <c r="I28" s="15"/>
     </row>
-    <row r="29" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21"/>
-      <c r="B29" s="15"/>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="15"/>
+      <c r="E29" s="14" t="n">
+        <v>0.0888</v>
+      </c>
+      <c r="F29" s="15" t="n">
+        <v>120</v>
+      </c>
       <c r="G29" s="14" t="n">
         <f aca="false">F29*E29</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="15"/>
+        <v>10.656</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>36</v>
+      </c>
       <c r="I29" s="15"/>
     </row>
     <row r="30" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1169,7 +1185,7 @@
       <c r="I30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="15"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -1197,151 +1213,141 @@
       <c r="I32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="14" t="n">
+        <f aca="false">F33*E33</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
     </row>
     <row r="34" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6"/>
-      <c r="F34" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G34" s="23" t="n">
-        <f aca="false">SUM(G6:G32)</f>
-        <v>578.7988</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
+      <c r="F35" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="23" t="n">
+        <f aca="false">SUM(G6:G33)</f>
+        <v>584.2388</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="A36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6"/>
+      <c r="A37" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B39" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D39" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E39" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F39" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G39" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H39" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="I39" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="12" t="n">
+    <row r="40" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="12" t="n">
         <v>79.99</v>
       </c>
-      <c r="E39" s="14" t="n">
-        <f aca="false">D39*D2</f>
+      <c r="E40" s="14" t="n">
+        <f aca="false">D40*D2</f>
         <v>108.7864</v>
       </c>
-      <c r="F39" s="11" t="n">
+      <c r="F40" s="11" t="n">
         <v>1</v>
-      </c>
-      <c r="G39" s="24" t="n">
-        <f aca="false">F39*E39</f>
-        <v>108.7864</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="15"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="n">
-        <v>2133</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="16" t="n">
-        <v>13.95</v>
-      </c>
-      <c r="F40" s="11" t="n">
-        <v>5</v>
       </c>
       <c r="G40" s="24" t="n">
         <f aca="false">F40*E40</f>
-        <v>69.75</v>
+        <v>108.7864</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="I40" s="15"/>
     </row>
     <row r="41" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="10" t="n">
+        <v>2133</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
       <c r="E41" s="16" t="n">
-        <v>11.8</v>
+        <v>13.95</v>
       </c>
       <c r="F41" s="11" t="n">
         <v>5</v>
       </c>
       <c r="G41" s="24" t="n">
         <f aca="false">F41*E41</f>
-        <v>59</v>
+        <v>69.75</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="I41" s="15"/>
     </row>
     <row r="42" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C42" s="13"/>
-      <c r="D42" s="12"/>
+      <c r="D42" s="13"/>
       <c r="E42" s="16" t="n">
-        <v>20</v>
+        <v>11.8</v>
       </c>
       <c r="F42" s="11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G42" s="24" t="n">
         <f aca="false">F42*E42</f>
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>21</v>
@@ -1349,83 +1355,83 @@
       <c r="I42" s="15"/>
     </row>
     <row r="43" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10" t="n">
-        <v>1405</v>
+      <c r="A43" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
+      <c r="D43" s="12"/>
       <c r="E43" s="16" t="n">
-        <v>0.75</v>
+        <v>20</v>
       </c>
       <c r="F43" s="11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G43" s="24" t="n">
         <f aca="false">F43*E43</f>
-        <v>3.75</v>
+        <v>20</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="I43" s="15"/>
     </row>
     <row r="44" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="s">
-        <v>70</v>
+      <c r="A44" s="10" t="n">
+        <v>1405</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C44" s="13"/>
-      <c r="D44" s="12" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="E44" s="14" t="n">
-        <f aca="false">D44*D2</f>
-        <v>1.7</v>
+      <c r="D44" s="13"/>
+      <c r="E44" s="16" t="n">
+        <v>0.75</v>
       </c>
       <c r="F44" s="11" t="n">
         <v>5</v>
       </c>
       <c r="G44" s="24" t="n">
         <f aca="false">F44*E44</f>
-        <v>8.5</v>
+        <v>3.75</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="I44" s="15"/>
     </row>
     <row r="45" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10" t="n">
-        <v>26171</v>
+      <c r="A45" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="16" t="n">
-        <v>12</v>
+      <c r="D45" s="12" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E45" s="14" t="n">
+        <f aca="false">D45*D2</f>
+        <v>1.7</v>
       </c>
       <c r="F45" s="11" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G45" s="24" t="n">
         <f aca="false">F45*E45</f>
-        <v>24</v>
+        <v>8.5</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="I45" s="15"/>
     </row>
     <row r="46" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10" t="s">
-        <v>73</v>
+      <c r="A46" s="10" t="n">
+        <v>26171</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>74</v>
@@ -1433,128 +1439,138 @@
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
       <c r="E46" s="16" t="n">
-        <v>64.99</v>
+        <v>12</v>
       </c>
       <c r="F46" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G46" s="24" t="n">
         <f aca="false">F46*E46</f>
-        <v>64.99</v>
+        <v>24</v>
       </c>
       <c r="H46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I46" s="15"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I46" s="15"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="10" t="n">
-        <v>1902</v>
-      </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
-      <c r="E47" s="14" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="F47" s="15" t="n">
+      <c r="E47" s="16" t="n">
+        <v>64.99</v>
+      </c>
+      <c r="F47" s="11" t="n">
         <v>1</v>
       </c>
       <c r="G47" s="24" t="n">
         <f aca="false">F47*E47</f>
-        <v>0.79</v>
+        <v>64.99</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="I47" s="15"/>
     </row>
     <row r="48" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="n">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
       <c r="E48" s="14" t="n">
-        <v>0.59</v>
+        <v>0.79</v>
       </c>
       <c r="F48" s="15" t="n">
         <v>1</v>
       </c>
       <c r="G48" s="24" t="n">
         <f aca="false">F48*E48</f>
-        <v>0.59</v>
-      </c>
-      <c r="H48" s="15" t="s">
-        <v>64</v>
+        <v>0.79</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="I48" s="15"/>
     </row>
     <row r="49" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="n">
-        <v>1901</v>
+        <v>1903</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
       <c r="E49" s="14" t="n">
-        <v>0.69</v>
+        <v>0.59</v>
       </c>
       <c r="F49" s="15" t="n">
         <v>1</v>
       </c>
       <c r="G49" s="24" t="n">
         <f aca="false">F49*E49</f>
-        <v>0.69</v>
+        <v>0.59</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I49" s="15"/>
     </row>
     <row r="50" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="n">
-        <v>1930</v>
+        <v>1901</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
       <c r="E50" s="14" t="n">
-        <v>5.95</v>
+        <v>0.69</v>
       </c>
       <c r="F50" s="15" t="n">
         <v>1</v>
       </c>
       <c r="G50" s="24" t="n">
         <f aca="false">F50*E50</f>
-        <v>5.95</v>
+        <v>0.69</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I50" s="15"/>
     </row>
     <row r="51" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="10"/>
-      <c r="B51" s="15"/>
+      <c r="A51" s="10" t="n">
+        <v>1930</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="15"/>
+      <c r="E51" s="14" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="F51" s="15" t="n">
+        <v>1</v>
+      </c>
       <c r="G51" s="24" t="n">
         <f aca="false">F51*E51</f>
-        <v>0</v>
-      </c>
-      <c r="H51" s="15"/>
+        <v>5.95</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>66</v>
+      </c>
       <c r="I51" s="15"/>
     </row>
     <row r="52" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1628,29 +1644,43 @@
       <c r="I56" s="15"/>
     </row>
     <row r="57" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6"/>
+      <c r="A57" s="10"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="24" t="n">
+        <f aca="false">F57*E57</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
     </row>
     <row r="58" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6"/>
-      <c r="F58" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G58" s="23" t="n">
-        <f aca="false">SUM(G39:G56)</f>
-        <v>366.7964</v>
-      </c>
     </row>
     <row r="59" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6"/>
+      <c r="F59" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G59" s="23" t="n">
+        <f aca="false">SUM(G40:G57)</f>
+        <v>366.7964</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6"/>
-      <c r="F60" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="G60" s="23" t="n">
-        <f aca="false">G58+G34</f>
-        <v>945.5952</v>
+    </row>
+    <row r="61" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="6"/>
+      <c r="F61" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G61" s="23" t="n">
+        <f aca="false">G59+G35</f>
+        <v>951.0352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM and printable parts
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
   <si>
     <t>GBP to USD</t>
   </si>
@@ -194,7 +194,7 @@
     <t>M3 fender washers</t>
   </si>
   <si>
-    <t>WC6360000A20000 </t>
+    <t>WC6360000A20000</t>
   </si>
   <si>
     <t>M6 fender washers</t>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>Female crimp pins; pack of 100</t>
+  </si>
+  <si>
+    <t>Printed Subtotal:</t>
   </si>
   <si>
     <t>Total:</t>
@@ -276,7 +279,7 @@
     <numFmt numFmtId="166" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -311,6 +314,13 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -361,7 +371,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -442,7 +452,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -459,6 +469,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -479,13 +497,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G64" activeCellId="0" sqref="G64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.3"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.5714285714286"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="98.030612244898"/>
@@ -511,6 +529,8 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="4"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
@@ -524,6 +544,8 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="4"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -535,6 +557,8 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="4"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
@@ -544,6 +568,8 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="4"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
@@ -1086,11 +1112,11 @@
         <v>0.1368</v>
       </c>
       <c r="F26" s="11" t="n">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="G26" s="14" t="n">
         <f aca="false">F26*E26</f>
-        <v>16.416</v>
+        <v>12.0384</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>36</v>
@@ -1147,7 +1173,7 @@
       <c r="I28" s="15"/>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="17" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="15" t="s">
@@ -1159,11 +1185,11 @@
         <v>0.0888</v>
       </c>
       <c r="F29" s="15" t="n">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="G29" s="14" t="n">
         <f aca="false">F29*E29</f>
-        <v>10.656</v>
+        <v>7.8144</v>
       </c>
       <c r="H29" s="15" t="s">
         <v>36</v>
@@ -1171,7 +1197,7 @@
       <c r="I29" s="15"/>
     </row>
     <row r="30" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="21"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="15"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
@@ -1228,27 +1254,65 @@
     </row>
     <row r="34" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
       <c r="F35" s="22" t="s">
         <v>61</v>
       </c>
       <c r="G35" s="23" t="n">
         <f aca="false">SUM(G6:G33)</f>
-        <v>584.2388</v>
-      </c>
+        <v>577.0196</v>
+      </c>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
+      <c r="I36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
+      <c r="I37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
+      <c r="I38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
@@ -1659,6 +1723,8 @@
     </row>
     <row r="58" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6"/>
+      <c r="F58" s="0"/>
+      <c r="G58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6"/>
@@ -1672,15 +1738,31 @@
     </row>
     <row r="60" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F60" s="0"/>
+      <c r="G60" s="0"/>
+    </row>
+    <row r="61" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6"/>
-      <c r="F61" s="22" t="s">
+      <c r="F61" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="G61" s="23" t="n">
-        <f aca="false">G59+G35</f>
-        <v>951.0352</v>
+      <c r="G61" s="26" t="n">
+        <v>131.97</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="6"/>
+      <c r="F62" s="0"/>
+      <c r="G62" s="0"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="6"/>
+      <c r="F63" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G63" s="23" t="n">
+        <f aca="false">G59+G35+G61</f>
+        <v>1075.786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>